<commit_message>
Use different method name for query in jxls template report with datasource specified in template
</commit_message>
<xml_diff>
--- a/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls11.xlsx
+++ b/src/art-parent/art/src/main/webapp/WEB-INF/work/templates/sample-jxls11.xlsx
@@ -65,7 +65,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="jdbc.query(1, 'select sum(city_id) value1 from cities')" var="results" lastCell="A4")</t>
+jx:each(items="jdbc.query2(1, 'select sum(city_id) value1 from cities')" var="results" lastCell="A4")</t>
         </r>
       </text>
     </comment>
@@ -89,7 +89,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="jdbc.query(1, 'select sum(region_id) value2 from cities')" var="results" lastCell="A5")</t>
+jx:each(items="jdbc.query2(1, 'select sum(region_id) value2 from cities')" var="results" lastCell="A5")</t>
         </r>
       </text>
     </comment>
@@ -479,7 +479,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>